<commit_message>
plot set locations and catch data
</commit_message>
<xml_diff>
--- a/data/taggingData/setData.xlsx
+++ b/data/taggingData/setData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="522">
   <si>
     <t>set</t>
   </si>
@@ -1591,6 +1591,9 @@
   </si>
   <si>
     <t>latDegreeStart</t>
+  </si>
+  <si>
+    <t>51.127</t>
   </si>
 </sst>
 </file>
@@ -2072,8 +2075,8 @@
   <dimension ref="A1:U134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7886,7 +7889,7 @@
         <v>48</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>319</v>
+        <v>521</v>
       </c>
       <c r="F92">
         <v>125</v>

</xml_diff>

<commit_message>
fix bugs in set locations
</commit_message>
<xml_diff>
--- a/data/taggingData/setData.xlsx
+++ b/data/taggingData/setData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="523">
   <si>
     <t>set</t>
   </si>
@@ -1594,6 +1594,9 @@
   </si>
   <si>
     <t>51.127</t>
+  </si>
+  <si>
+    <t>35.092</t>
   </si>
 </sst>
 </file>
@@ -2076,7 +2079,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E92" sqref="E92"/>
+      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6626,7 +6629,7 @@
         <v>125</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>289</v>
+        <v>522</v>
       </c>
       <c r="H72">
         <v>48</v>

</xml_diff>

<commit_message>
correct set locations and update returned tags
</commit_message>
<xml_diff>
--- a/data/taggingData/setData.xlsx
+++ b/data/taggingData/setData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2777" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2770" uniqueCount="815">
   <si>
     <t>set</t>
   </si>
@@ -2049,9 +2049,6 @@
     <t>48.896</t>
   </si>
   <si>
-    <t>32.021</t>
-  </si>
-  <si>
     <t>32.297</t>
   </si>
   <si>
@@ -2463,18 +2460,9 @@
     <t>50.125</t>
   </si>
   <si>
-    <t>check start long</t>
-  </si>
-  <si>
     <t>48.395</t>
   </si>
   <si>
-    <t>51.902</t>
-  </si>
-  <si>
-    <t>check start lat</t>
-  </si>
-  <si>
     <t>37.328</t>
   </si>
   <si>
@@ -2484,16 +2472,7 @@
     <t>40.511</t>
   </si>
   <si>
-    <t>check start coords</t>
-  </si>
-  <si>
     <t>46.437</t>
-  </si>
-  <si>
-    <t>CHECK START LAT/LONG</t>
-  </si>
-  <si>
-    <t>CHECK START LONG</t>
   </si>
 </sst>
 </file>
@@ -3242,9 +3221,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U221"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U175" sqref="U175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4571,7 +4550,7 @@
         <v>48</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="J21">
         <v>125</v>
@@ -4622,7 +4601,7 @@
         <v>48</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="F22">
         <v>125</v>
@@ -4670,7 +4649,7 @@
         <v>39</v>
       </c>
       <c r="U22" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -8351,7 +8330,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_080</v>
@@ -8414,7 +8393,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_081</v>
@@ -8477,7 +8456,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_082</v>
@@ -8540,7 +8519,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_083</v>
@@ -8603,7 +8582,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_084</v>
@@ -8666,7 +8645,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_085</v>
@@ -8729,7 +8708,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_086</v>
@@ -8792,7 +8771,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_087</v>
@@ -8854,11 +8833,8 @@
       <c r="T88" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="U88" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_088</v>
@@ -8921,7 +8897,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_089</v>
@@ -8984,7 +8960,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_090</v>
@@ -9047,7 +9023,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_091</v>
@@ -9110,7 +9086,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_092</v>
@@ -9173,7 +9149,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_093</v>
@@ -9236,7 +9212,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_094</v>
@@ -9299,7 +9275,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" t="str">
         <f t="shared" si="1"/>
         <v>CT2019_095</v>
@@ -10283,7 +10259,7 @@
         <v>125</v>
       </c>
       <c r="K111" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="L111" s="3" t="s">
         <v>404</v>
@@ -10311,9 +10287,6 @@
       </c>
       <c r="T111" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="U111" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.3">
@@ -10337,7 +10310,7 @@
         <v>125</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="H112">
         <v>48</v>
@@ -10377,9 +10350,6 @@
       </c>
       <c r="T112" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="U112" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.3">
@@ -10415,7 +10385,7 @@
         <v>125</v>
       </c>
       <c r="K113" s="3" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="L113" s="3" t="s">
         <v>407</v>
@@ -10466,7 +10436,7 @@
         <v>125</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="H114">
         <v>48</v>
@@ -10506,9 +10476,6 @@
       </c>
       <c r="T114" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="U114" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.3">
@@ -10607,7 +10574,7 @@
         <v>125</v>
       </c>
       <c r="K116" s="3" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="L116" s="3" t="s">
         <v>410</v>
@@ -10658,7 +10625,7 @@
         <v>125</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="H117">
         <v>48</v>
@@ -10698,9 +10665,6 @@
       </c>
       <c r="T117" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="U117" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.3">
@@ -12031,9 +11995,6 @@
       <c r="T138" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="U138" t="s">
-        <v>821</v>
-      </c>
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A139" t="str">
@@ -14018,7 +13979,7 @@
         <v>48</v>
       </c>
       <c r="I170" s="3" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="J170">
         <v>125</v>
@@ -14069,7 +14030,7 @@
         <v>48</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="F171">
         <v>125</v>
@@ -14135,13 +14096,13 @@
         <v>48</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>813</v>
+        <v>634</v>
       </c>
       <c r="F172">
         <v>125</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>673</v>
+        <v>635</v>
       </c>
       <c r="H172">
         <v>48</v>
@@ -14153,7 +14114,7 @@
         <v>125</v>
       </c>
       <c r="K172" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="L172" s="3" t="s">
         <v>176</v>
@@ -14181,9 +14142,6 @@
       </c>
       <c r="T172" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="U172" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.3">
@@ -14207,7 +14165,7 @@
         <v>125</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H173">
         <v>48</v>
@@ -14219,7 +14177,7 @@
         <v>125</v>
       </c>
       <c r="K173" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="L173" s="3" t="s">
         <v>239</v>
@@ -14270,7 +14228,7 @@
         <v>125</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="H174">
         <v>48</v>
@@ -14282,7 +14240,7 @@
         <v>125</v>
       </c>
       <c r="K174" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="L174" s="3" t="s">
         <v>95</v>
@@ -14333,7 +14291,7 @@
         <v>125</v>
       </c>
       <c r="G175" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H175">
         <v>48</v>
@@ -14345,7 +14303,7 @@
         <v>125</v>
       </c>
       <c r="K175" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="L175" s="3" t="s">
         <v>96</v>
@@ -14396,7 +14354,7 @@
         <v>125</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H176">
         <v>48</v>
@@ -14408,7 +14366,7 @@
         <v>125</v>
       </c>
       <c r="K176" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="L176" s="3" t="s">
         <v>97</v>
@@ -14459,7 +14417,7 @@
         <v>125</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H177">
         <v>48</v>
@@ -14471,7 +14429,7 @@
         <v>125</v>
       </c>
       <c r="K177" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="L177" s="3" t="s">
         <v>20</v>
@@ -14522,7 +14480,7 @@
         <v>125</v>
       </c>
       <c r="G178" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H178">
         <v>48</v>
@@ -14534,7 +14492,7 @@
         <v>125</v>
       </c>
       <c r="K178" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="L178" s="3" t="s">
         <v>240</v>
@@ -14585,7 +14543,7 @@
         <v>125</v>
       </c>
       <c r="G179" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="H179">
         <v>48</v>
@@ -14597,7 +14555,7 @@
         <v>125</v>
       </c>
       <c r="K179" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="L179" s="3" t="s">
         <v>241</v>
@@ -14648,7 +14606,7 @@
         <v>125</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H180">
         <v>48</v>
@@ -14660,7 +14618,7 @@
         <v>125</v>
       </c>
       <c r="K180" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="L180" s="3" t="s">
         <v>28</v>
@@ -14711,7 +14669,7 @@
         <v>125</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H181">
         <v>48</v>
@@ -14723,7 +14681,7 @@
         <v>125</v>
       </c>
       <c r="K181" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="L181" s="3" t="s">
         <v>182</v>
@@ -14774,7 +14732,7 @@
         <v>125</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H182">
         <v>48</v>
@@ -14786,7 +14744,7 @@
         <v>125</v>
       </c>
       <c r="K182" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="L182" s="3" t="s">
         <v>101</v>
@@ -14837,7 +14795,7 @@
         <v>125</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H183">
         <v>48</v>
@@ -14849,7 +14807,7 @@
         <v>125</v>
       </c>
       <c r="K183" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="L183" s="3" t="s">
         <v>34</v>
@@ -14900,7 +14858,7 @@
         <v>125</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H184">
         <v>48</v>
@@ -14912,7 +14870,7 @@
         <v>125</v>
       </c>
       <c r="K184" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="L184" s="3" t="s">
         <v>183</v>
@@ -14963,7 +14921,7 @@
         <v>125</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H185">
         <v>48</v>
@@ -14975,7 +14933,7 @@
         <v>125</v>
       </c>
       <c r="K185" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="L185" s="3" t="s">
         <v>184</v>
@@ -15026,7 +14984,7 @@
         <v>125</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H186">
         <v>48</v>
@@ -15038,7 +14996,7 @@
         <v>125</v>
       </c>
       <c r="K186" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="L186" s="3" t="s">
         <v>44</v>
@@ -15089,19 +15047,19 @@
         <v>125</v>
       </c>
       <c r="G187" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="H187">
+        <v>48</v>
+      </c>
+      <c r="I187" s="3" t="s">
         <v>688</v>
       </c>
-      <c r="H187">
-        <v>48</v>
-      </c>
-      <c r="I187" s="3" t="s">
+      <c r="J187">
+        <v>125</v>
+      </c>
+      <c r="K187" s="3" t="s">
         <v>689</v>
-      </c>
-      <c r="J187">
-        <v>125</v>
-      </c>
-      <c r="K187" s="3" t="s">
-        <v>690</v>
       </c>
       <c r="L187" s="3" t="s">
         <v>66</v>
@@ -15131,7 +15089,7 @@
         <v>38</v>
       </c>
       <c r="U187" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.3">
@@ -15140,34 +15098,34 @@
         <v>CT2019_187</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C188" t="s">
+        <v>709</v>
+      </c>
+      <c r="D188">
+        <v>48</v>
+      </c>
+      <c r="E188" s="3" t="s">
         <v>710</v>
       </c>
-      <c r="D188">
-        <v>48</v>
-      </c>
-      <c r="E188" s="3" t="s">
+      <c r="F188">
+        <v>125</v>
+      </c>
+      <c r="G188" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="H188">
+        <v>48</v>
+      </c>
+      <c r="I188" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="F188">
-        <v>125</v>
-      </c>
-      <c r="G188" s="3" t="s">
+      <c r="J188">
+        <v>125</v>
+      </c>
+      <c r="K188" s="3" t="s">
         <v>730</v>
-      </c>
-      <c r="H188">
-        <v>48</v>
-      </c>
-      <c r="I188" s="3" t="s">
-        <v>712</v>
-      </c>
-      <c r="J188">
-        <v>125</v>
-      </c>
-      <c r="K188" s="3" t="s">
-        <v>731</v>
       </c>
       <c r="L188" s="3" t="s">
         <v>19</v>
@@ -15203,34 +15161,34 @@
         <v>CT2019_188</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C189" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D189">
         <v>48</v>
       </c>
       <c r="E189" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="F189">
+        <v>125</v>
+      </c>
+      <c r="G189" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="H189">
+        <v>48</v>
+      </c>
+      <c r="I189" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="F189">
-        <v>125</v>
-      </c>
-      <c r="G189" s="3" t="s">
+      <c r="J189">
+        <v>125</v>
+      </c>
+      <c r="K189" s="3" t="s">
         <v>731</v>
-      </c>
-      <c r="H189">
-        <v>48</v>
-      </c>
-      <c r="I189" s="3" t="s">
-        <v>713</v>
-      </c>
-      <c r="J189">
-        <v>125</v>
-      </c>
-      <c r="K189" s="3" t="s">
-        <v>732</v>
       </c>
       <c r="L189" s="3" t="s">
         <v>20</v>
@@ -15266,34 +15224,34 @@
         <v>CT2019_189</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C190" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D190">
         <v>48</v>
       </c>
       <c r="E190" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="F190">
+        <v>125</v>
+      </c>
+      <c r="G190" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="H190">
+        <v>48</v>
+      </c>
+      <c r="I190" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="F190">
-        <v>125</v>
-      </c>
-      <c r="G190" s="3" t="s">
+      <c r="J190">
+        <v>125</v>
+      </c>
+      <c r="K190" s="3" t="s">
         <v>732</v>
-      </c>
-      <c r="H190">
-        <v>48</v>
-      </c>
-      <c r="I190" s="3" t="s">
-        <v>714</v>
-      </c>
-      <c r="J190">
-        <v>125</v>
-      </c>
-      <c r="K190" s="3" t="s">
-        <v>733</v>
       </c>
       <c r="L190" s="3" t="s">
         <v>240</v>
@@ -15329,34 +15287,34 @@
         <v>CT2019_190</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C191" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D191">
         <v>48</v>
       </c>
       <c r="E191" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="F191">
+        <v>125</v>
+      </c>
+      <c r="G191" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="H191">
+        <v>48</v>
+      </c>
+      <c r="I191" s="3" t="s">
         <v>714</v>
       </c>
-      <c r="F191">
-        <v>125</v>
-      </c>
-      <c r="G191" s="3" t="s">
+      <c r="J191">
+        <v>125</v>
+      </c>
+      <c r="K191" s="3" t="s">
         <v>733</v>
-      </c>
-      <c r="H191">
-        <v>48</v>
-      </c>
-      <c r="I191" s="3" t="s">
-        <v>715</v>
-      </c>
-      <c r="J191">
-        <v>125</v>
-      </c>
-      <c r="K191" s="3" t="s">
-        <v>734</v>
       </c>
       <c r="L191" s="3" t="s">
         <v>241</v>
@@ -15392,34 +15350,34 @@
         <v>CT2019_191</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C192" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D192">
         <v>48</v>
       </c>
       <c r="E192" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="F192">
+        <v>125</v>
+      </c>
+      <c r="G192" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="H192">
+        <v>48</v>
+      </c>
+      <c r="I192" s="3" t="s">
         <v>715</v>
       </c>
-      <c r="F192">
-        <v>125</v>
-      </c>
-      <c r="G192" s="3" t="s">
+      <c r="J192">
+        <v>125</v>
+      </c>
+      <c r="K192" s="3" t="s">
         <v>734</v>
-      </c>
-      <c r="H192">
-        <v>48</v>
-      </c>
-      <c r="I192" s="3" t="s">
-        <v>716</v>
-      </c>
-      <c r="J192">
-        <v>125</v>
-      </c>
-      <c r="K192" s="3" t="s">
-        <v>735</v>
       </c>
       <c r="L192" s="3" t="s">
         <v>28</v>
@@ -15455,34 +15413,34 @@
         <v>CT2019_192</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C193" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D193">
         <v>48</v>
       </c>
       <c r="E193" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="F193">
+        <v>125</v>
+      </c>
+      <c r="G193" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="H193">
+        <v>48</v>
+      </c>
+      <c r="I193" s="3" t="s">
         <v>716</v>
       </c>
-      <c r="F193">
-        <v>125</v>
-      </c>
-      <c r="G193" s="3" t="s">
+      <c r="J193">
+        <v>125</v>
+      </c>
+      <c r="K193" s="3" t="s">
         <v>735</v>
-      </c>
-      <c r="H193">
-        <v>48</v>
-      </c>
-      <c r="I193" s="3" t="s">
-        <v>717</v>
-      </c>
-      <c r="J193">
-        <v>125</v>
-      </c>
-      <c r="K193" s="3" t="s">
-        <v>736</v>
       </c>
       <c r="L193" s="3" t="s">
         <v>182</v>
@@ -15518,34 +15476,34 @@
         <v>CT2019_193</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C194" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D194">
         <v>48</v>
       </c>
       <c r="E194" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="F194">
+        <v>125</v>
+      </c>
+      <c r="G194" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="H194">
+        <v>48</v>
+      </c>
+      <c r="I194" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="F194">
-        <v>125</v>
-      </c>
-      <c r="G194" s="3" t="s">
+      <c r="J194">
+        <v>125</v>
+      </c>
+      <c r="K194" s="3" t="s">
         <v>736</v>
-      </c>
-      <c r="H194">
-        <v>48</v>
-      </c>
-      <c r="I194" s="3" t="s">
-        <v>718</v>
-      </c>
-      <c r="J194">
-        <v>125</v>
-      </c>
-      <c r="K194" s="3" t="s">
-        <v>737</v>
       </c>
       <c r="L194" s="3" t="s">
         <v>101</v>
@@ -15554,7 +15512,7 @@
         <v>2</v>
       </c>
       <c r="N194" s="3" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="O194" s="3" t="s">
         <v>10</v>
@@ -15575,7 +15533,7 @@
         <v>37</v>
       </c>
       <c r="U194" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.3">
@@ -15584,34 +15542,34 @@
         <v>CT2019_194</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C195" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D195">
         <v>48</v>
       </c>
       <c r="E195" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="F195">
+        <v>125</v>
+      </c>
+      <c r="G195" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="H195">
+        <v>48</v>
+      </c>
+      <c r="I195" s="3" t="s">
         <v>718</v>
       </c>
-      <c r="F195">
-        <v>125</v>
-      </c>
-      <c r="G195" s="3" t="s">
+      <c r="J195">
+        <v>125</v>
+      </c>
+      <c r="K195" s="3" t="s">
         <v>737</v>
-      </c>
-      <c r="H195">
-        <v>48</v>
-      </c>
-      <c r="I195" s="3" t="s">
-        <v>719</v>
-      </c>
-      <c r="J195">
-        <v>125</v>
-      </c>
-      <c r="K195" s="3" t="s">
-        <v>738</v>
       </c>
       <c r="L195" s="3" t="s">
         <v>34</v>
@@ -15620,7 +15578,7 @@
         <v>2</v>
       </c>
       <c r="N195" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="O195" s="3" t="s">
         <v>10</v>
@@ -15641,7 +15599,7 @@
         <v>37</v>
       </c>
       <c r="U195" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="196" spans="1:21" x14ac:dyDescent="0.3">
@@ -15650,34 +15608,34 @@
         <v>CT2019_195</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C196" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D196">
         <v>48</v>
       </c>
       <c r="E196" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="F196">
+        <v>125</v>
+      </c>
+      <c r="G196" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="H196">
+        <v>48</v>
+      </c>
+      <c r="I196" s="3" t="s">
         <v>719</v>
       </c>
-      <c r="F196">
-        <v>125</v>
-      </c>
-      <c r="G196" s="3" t="s">
+      <c r="J196">
+        <v>125</v>
+      </c>
+      <c r="K196" s="3" t="s">
         <v>738</v>
-      </c>
-      <c r="H196">
-        <v>48</v>
-      </c>
-      <c r="I196" s="3" t="s">
-        <v>720</v>
-      </c>
-      <c r="J196">
-        <v>125</v>
-      </c>
-      <c r="K196" s="3" t="s">
-        <v>739</v>
       </c>
       <c r="L196" s="3" t="s">
         <v>183</v>
@@ -15686,7 +15644,7 @@
         <v>2</v>
       </c>
       <c r="N196" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="O196" s="3" t="s">
         <v>10</v>
@@ -15707,7 +15665,7 @@
         <v>37</v>
       </c>
       <c r="U196" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.3">
@@ -15716,34 +15674,34 @@
         <v>CT2019_196</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C197" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D197">
         <v>48</v>
       </c>
       <c r="E197" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="F197">
+        <v>125</v>
+      </c>
+      <c r="G197" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="H197">
+        <v>48</v>
+      </c>
+      <c r="I197" s="3" t="s">
         <v>720</v>
       </c>
-      <c r="F197">
-        <v>125</v>
-      </c>
-      <c r="G197" s="3" t="s">
+      <c r="J197">
+        <v>125</v>
+      </c>
+      <c r="K197" s="3" t="s">
         <v>739</v>
-      </c>
-      <c r="H197">
-        <v>48</v>
-      </c>
-      <c r="I197" s="3" t="s">
-        <v>721</v>
-      </c>
-      <c r="J197">
-        <v>125</v>
-      </c>
-      <c r="K197" s="3" t="s">
-        <v>740</v>
       </c>
       <c r="L197" s="3" t="s">
         <v>184</v>
@@ -15752,7 +15710,7 @@
         <v>2</v>
       </c>
       <c r="N197" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="O197" s="3" t="s">
         <v>10</v>
@@ -15773,7 +15731,7 @@
         <v>37</v>
       </c>
       <c r="U197" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.3">
@@ -15782,34 +15740,34 @@
         <v>CT2019_197</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C198" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D198">
         <v>48</v>
       </c>
       <c r="E198" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="F198">
+        <v>125</v>
+      </c>
+      <c r="G198" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="H198">
+        <v>48</v>
+      </c>
+      <c r="I198" s="3" t="s">
         <v>721</v>
       </c>
-      <c r="F198">
-        <v>125</v>
-      </c>
-      <c r="G198" s="3" t="s">
+      <c r="J198">
+        <v>125</v>
+      </c>
+      <c r="K198" s="3" t="s">
         <v>740</v>
-      </c>
-      <c r="H198">
-        <v>48</v>
-      </c>
-      <c r="I198" s="3" t="s">
-        <v>722</v>
-      </c>
-      <c r="J198">
-        <v>125</v>
-      </c>
-      <c r="K198" s="3" t="s">
-        <v>741</v>
       </c>
       <c r="L198" s="3" t="s">
         <v>44</v>
@@ -15818,7 +15776,7 @@
         <v>2</v>
       </c>
       <c r="N198" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="O198" s="3" t="s">
         <v>10</v>
@@ -15839,7 +15797,7 @@
         <v>37</v>
       </c>
       <c r="U198" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.3">
@@ -15848,34 +15806,34 @@
         <v>CT2019_198</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C199" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D199">
         <v>48</v>
       </c>
       <c r="E199" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="F199">
+        <v>125</v>
+      </c>
+      <c r="G199" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="H199">
+        <v>48</v>
+      </c>
+      <c r="I199" s="3" t="s">
         <v>722</v>
       </c>
-      <c r="F199">
-        <v>125</v>
-      </c>
-      <c r="G199" s="3" t="s">
+      <c r="J199">
+        <v>125</v>
+      </c>
+      <c r="K199" s="3" t="s">
         <v>741</v>
-      </c>
-      <c r="H199">
-        <v>48</v>
-      </c>
-      <c r="I199" s="3" t="s">
-        <v>723</v>
-      </c>
-      <c r="J199">
-        <v>125</v>
-      </c>
-      <c r="K199" s="3" t="s">
-        <v>742</v>
       </c>
       <c r="L199" s="3" t="s">
         <v>66</v>
@@ -15884,7 +15842,7 @@
         <v>2</v>
       </c>
       <c r="N199" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="O199" s="3" t="s">
         <v>10</v>
@@ -15905,7 +15863,7 @@
         <v>37</v>
       </c>
       <c r="U199" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.3">
@@ -15914,34 +15872,34 @@
         <v>CT2019_199</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C200" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D200">
         <v>48</v>
       </c>
       <c r="E200" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="F200">
+        <v>125</v>
+      </c>
+      <c r="G200" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="H200">
+        <v>48</v>
+      </c>
+      <c r="I200" s="3" t="s">
         <v>723</v>
       </c>
-      <c r="F200">
-        <v>125</v>
-      </c>
-      <c r="G200" s="3" t="s">
+      <c r="J200">
+        <v>125</v>
+      </c>
+      <c r="K200" s="3" t="s">
         <v>742</v>
-      </c>
-      <c r="H200">
-        <v>48</v>
-      </c>
-      <c r="I200" s="3" t="s">
-        <v>724</v>
-      </c>
-      <c r="J200">
-        <v>125</v>
-      </c>
-      <c r="K200" s="3" t="s">
-        <v>743</v>
       </c>
       <c r="L200" s="3" t="s">
         <v>67</v>
@@ -15950,7 +15908,7 @@
         <v>2</v>
       </c>
       <c r="N200" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="O200" s="3" t="s">
         <v>10</v>
@@ -15971,7 +15929,7 @@
         <v>37</v>
       </c>
       <c r="U200" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.3">
@@ -15980,34 +15938,34 @@
         <v>CT2019_200</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C201" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D201">
         <v>48</v>
       </c>
       <c r="E201" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="F201">
+        <v>125</v>
+      </c>
+      <c r="G201" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="H201">
+        <v>48</v>
+      </c>
+      <c r="I201" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="F201">
-        <v>125</v>
-      </c>
-      <c r="G201" s="3" t="s">
+      <c r="J201">
+        <v>125</v>
+      </c>
+      <c r="K201" s="3" t="s">
         <v>743</v>
-      </c>
-      <c r="H201">
-        <v>48</v>
-      </c>
-      <c r="I201" s="3" t="s">
-        <v>725</v>
-      </c>
-      <c r="J201">
-        <v>125</v>
-      </c>
-      <c r="K201" s="3" t="s">
-        <v>744</v>
       </c>
       <c r="L201" s="3" t="s">
         <v>68</v>
@@ -16016,7 +15974,7 @@
         <v>2</v>
       </c>
       <c r="N201" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="O201" s="3" t="s">
         <v>10</v>
@@ -16037,7 +15995,7 @@
         <v>37</v>
       </c>
       <c r="U201" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.3">
@@ -16046,34 +16004,34 @@
         <v>CT2019_201</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C202" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D202">
         <v>48</v>
       </c>
       <c r="E202" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="F202">
+        <v>125</v>
+      </c>
+      <c r="G202" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="H202">
+        <v>48</v>
+      </c>
+      <c r="I202" s="3" t="s">
         <v>725</v>
       </c>
-      <c r="F202">
-        <v>125</v>
-      </c>
-      <c r="G202" s="3" t="s">
+      <c r="J202">
+        <v>125</v>
+      </c>
+      <c r="K202" s="3" t="s">
         <v>744</v>
-      </c>
-      <c r="H202">
-        <v>48</v>
-      </c>
-      <c r="I202" s="3" t="s">
-        <v>726</v>
-      </c>
-      <c r="J202">
-        <v>125</v>
-      </c>
-      <c r="K202" s="3" t="s">
-        <v>745</v>
       </c>
       <c r="L202" s="3" t="s">
         <v>69</v>
@@ -16082,7 +16040,7 @@
         <v>2</v>
       </c>
       <c r="N202" s="3" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="O202" s="3" t="s">
         <v>10</v>
@@ -16103,7 +16061,7 @@
         <v>37</v>
       </c>
       <c r="U202" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.3">
@@ -16112,34 +16070,34 @@
         <v>CT2019_202</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C203" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D203">
         <v>48</v>
       </c>
       <c r="E203" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="F203">
+        <v>125</v>
+      </c>
+      <c r="G203" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="H203">
+        <v>48</v>
+      </c>
+      <c r="I203" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="F203">
-        <v>125</v>
-      </c>
-      <c r="G203" s="3" t="s">
+      <c r="J203">
+        <v>125</v>
+      </c>
+      <c r="K203" s="3" t="s">
         <v>745</v>
-      </c>
-      <c r="H203">
-        <v>48</v>
-      </c>
-      <c r="I203" s="3" t="s">
-        <v>727</v>
-      </c>
-      <c r="J203">
-        <v>125</v>
-      </c>
-      <c r="K203" s="3" t="s">
-        <v>746</v>
       </c>
       <c r="L203" s="3" t="s">
         <v>185</v>
@@ -16148,7 +16106,7 @@
         <v>2</v>
       </c>
       <c r="N203" s="3" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="O203" s="3" t="s">
         <v>10</v>
@@ -16169,7 +16127,7 @@
         <v>37</v>
       </c>
       <c r="U203" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.3">
@@ -16178,34 +16136,34 @@
         <v>CT2019_203</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C204" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D204">
         <v>48</v>
       </c>
       <c r="E204" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="F204">
+        <v>125</v>
+      </c>
+      <c r="G204" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="H204">
+        <v>48</v>
+      </c>
+      <c r="I204" s="3" t="s">
         <v>727</v>
       </c>
-      <c r="F204">
-        <v>125</v>
-      </c>
-      <c r="G204" s="3" t="s">
+      <c r="J204">
+        <v>125</v>
+      </c>
+      <c r="K204" s="3" t="s">
         <v>746</v>
-      </c>
-      <c r="H204">
-        <v>48</v>
-      </c>
-      <c r="I204" s="3" t="s">
-        <v>728</v>
-      </c>
-      <c r="J204">
-        <v>125</v>
-      </c>
-      <c r="K204" s="3" t="s">
-        <v>747</v>
       </c>
       <c r="L204" s="3" t="s">
         <v>71</v>
@@ -16214,7 +16172,7 @@
         <v>2</v>
       </c>
       <c r="N204" s="3" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="O204" s="3" t="s">
         <v>10</v>
@@ -16235,7 +16193,7 @@
         <v>38</v>
       </c>
       <c r="U204" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.3">
@@ -16244,43 +16202,43 @@
         <v>CT2019_204</v>
       </c>
       <c r="B205" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="C205" t="s">
         <v>709</v>
       </c>
-      <c r="C205" t="s">
-        <v>710</v>
-      </c>
       <c r="D205">
         <v>48</v>
       </c>
       <c r="E205" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="F205">
+        <v>125</v>
+      </c>
+      <c r="G205" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="H205">
+        <v>48</v>
+      </c>
+      <c r="I205" s="3" t="s">
         <v>728</v>
       </c>
-      <c r="F205">
-        <v>125</v>
-      </c>
-      <c r="G205" s="3" t="s">
+      <c r="J205">
+        <v>125</v>
+      </c>
+      <c r="K205" s="3" t="s">
         <v>747</v>
       </c>
-      <c r="H205">
-        <v>48</v>
-      </c>
-      <c r="I205" s="3" t="s">
-        <v>729</v>
-      </c>
-      <c r="J205">
-        <v>125</v>
-      </c>
-      <c r="K205" s="3" t="s">
+      <c r="L205" s="3" t="s">
         <v>748</v>
       </c>
-      <c r="L205" s="3" t="s">
+      <c r="M205">
+        <v>2</v>
+      </c>
+      <c r="N205" s="3" t="s">
         <v>749</v>
-      </c>
-      <c r="M205">
-        <v>2</v>
-      </c>
-      <c r="N205" s="3" t="s">
-        <v>750</v>
       </c>
       <c r="O205" s="3" t="s">
         <v>10</v>
@@ -16301,7 +16259,7 @@
         <v>37</v>
       </c>
       <c r="U205" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.3">
@@ -16310,34 +16268,34 @@
         <v>CT2019_205</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C206" t="s">
+        <v>770</v>
+      </c>
+      <c r="D206">
+        <v>48</v>
+      </c>
+      <c r="E206" s="3" t="s">
         <v>771</v>
       </c>
-      <c r="D206">
-        <v>48</v>
-      </c>
-      <c r="E206" s="3" t="s">
+      <c r="F206">
+        <v>125</v>
+      </c>
+      <c r="G206" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="H206">
+        <v>48</v>
+      </c>
+      <c r="I206" s="3" t="s">
         <v>772</v>
       </c>
-      <c r="F206">
-        <v>125</v>
-      </c>
-      <c r="G206" s="3" t="s">
+      <c r="J206">
+        <v>125</v>
+      </c>
+      <c r="K206" s="3" t="s">
         <v>789</v>
-      </c>
-      <c r="H206">
-        <v>48</v>
-      </c>
-      <c r="I206" s="3" t="s">
-        <v>773</v>
-      </c>
-      <c r="J206">
-        <v>125</v>
-      </c>
-      <c r="K206" s="3" t="s">
-        <v>790</v>
       </c>
       <c r="L206" s="3" t="s">
         <v>486</v>
@@ -16367,7 +16325,7 @@
         <v>38</v>
       </c>
       <c r="U206" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.3">
@@ -16376,34 +16334,34 @@
         <v>CT2019_206</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C207" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D207">
         <v>48</v>
       </c>
       <c r="E207" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="F207">
+        <v>125</v>
+      </c>
+      <c r="G207" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="H207">
+        <v>48</v>
+      </c>
+      <c r="I207" s="3" t="s">
         <v>773</v>
       </c>
-      <c r="F207">
-        <v>125</v>
-      </c>
-      <c r="G207" s="3" t="s">
+      <c r="J207">
+        <v>125</v>
+      </c>
+      <c r="K207" s="3" t="s">
         <v>790</v>
-      </c>
-      <c r="H207">
-        <v>48</v>
-      </c>
-      <c r="I207" s="3" t="s">
-        <v>774</v>
-      </c>
-      <c r="J207">
-        <v>125</v>
-      </c>
-      <c r="K207" s="3" t="s">
-        <v>791</v>
       </c>
       <c r="L207" s="3" t="s">
         <v>292</v>
@@ -16433,7 +16391,7 @@
         <v>38</v>
       </c>
       <c r="U207" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.3">
@@ -16442,34 +16400,34 @@
         <v>CT2019_207</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C208" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D208">
         <v>48</v>
       </c>
       <c r="E208" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="F208">
+        <v>125</v>
+      </c>
+      <c r="G208" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="H208">
+        <v>48</v>
+      </c>
+      <c r="I208" s="3" t="s">
         <v>774</v>
       </c>
-      <c r="F208">
-        <v>125</v>
-      </c>
-      <c r="G208" s="3" t="s">
+      <c r="J208">
+        <v>125</v>
+      </c>
+      <c r="K208" s="3" t="s">
         <v>791</v>
-      </c>
-      <c r="H208">
-        <v>48</v>
-      </c>
-      <c r="I208" s="3" t="s">
-        <v>775</v>
-      </c>
-      <c r="J208">
-        <v>125</v>
-      </c>
-      <c r="K208" s="3" t="s">
-        <v>792</v>
       </c>
       <c r="L208" s="3" t="s">
         <v>239</v>
@@ -16499,7 +16457,7 @@
         <v>38</v>
       </c>
       <c r="U208" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.3">
@@ -16508,34 +16466,34 @@
         <v>CT2019_208</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C209" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D209">
         <v>48</v>
       </c>
       <c r="E209" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="F209">
+        <v>125</v>
+      </c>
+      <c r="G209" s="3" t="s">
+        <v>791</v>
+      </c>
+      <c r="H209">
+        <v>48</v>
+      </c>
+      <c r="I209" s="3" t="s">
         <v>775</v>
       </c>
-      <c r="F209">
-        <v>125</v>
-      </c>
-      <c r="G209" s="3" t="s">
+      <c r="J209">
+        <v>125</v>
+      </c>
+      <c r="K209" s="3" t="s">
         <v>792</v>
-      </c>
-      <c r="H209">
-        <v>48</v>
-      </c>
-      <c r="I209" s="3" t="s">
-        <v>776</v>
-      </c>
-      <c r="J209">
-        <v>125</v>
-      </c>
-      <c r="K209" s="3" t="s">
-        <v>793</v>
       </c>
       <c r="L209" s="3" t="s">
         <v>95</v>
@@ -16565,7 +16523,7 @@
         <v>38</v>
       </c>
       <c r="U209" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="210" spans="1:21" x14ac:dyDescent="0.3">
@@ -16574,34 +16532,34 @@
         <v>CT2019_209</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C210" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D210">
         <v>48</v>
       </c>
       <c r="E210" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="F210">
+        <v>125</v>
+      </c>
+      <c r="G210" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="H210">
+        <v>48</v>
+      </c>
+      <c r="I210" s="3" t="s">
         <v>776</v>
       </c>
-      <c r="F210">
-        <v>125</v>
-      </c>
-      <c r="G210" s="3" t="s">
+      <c r="J210">
+        <v>125</v>
+      </c>
+      <c r="K210" s="3" t="s">
         <v>793</v>
-      </c>
-      <c r="H210">
-        <v>48</v>
-      </c>
-      <c r="I210" s="3" t="s">
-        <v>777</v>
-      </c>
-      <c r="J210">
-        <v>125</v>
-      </c>
-      <c r="K210" s="3" t="s">
-        <v>794</v>
       </c>
       <c r="L210" s="3" t="s">
         <v>96</v>
@@ -16631,7 +16589,7 @@
         <v>38</v>
       </c>
       <c r="U210" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.3">
@@ -16640,34 +16598,34 @@
         <v>CT2019_210</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C211" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D211">
         <v>48</v>
       </c>
       <c r="E211" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="F211">
+        <v>125</v>
+      </c>
+      <c r="G211" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="H211">
+        <v>48</v>
+      </c>
+      <c r="I211" s="3" t="s">
         <v>777</v>
       </c>
-      <c r="F211">
-        <v>125</v>
-      </c>
-      <c r="G211" s="3" t="s">
+      <c r="J211">
+        <v>125</v>
+      </c>
+      <c r="K211" s="3" t="s">
         <v>794</v>
-      </c>
-      <c r="H211">
-        <v>48</v>
-      </c>
-      <c r="I211" s="3" t="s">
-        <v>778</v>
-      </c>
-      <c r="J211">
-        <v>125</v>
-      </c>
-      <c r="K211" s="3" t="s">
-        <v>795</v>
       </c>
       <c r="L211" s="3" t="s">
         <v>97</v>
@@ -16697,7 +16655,7 @@
         <v>38</v>
       </c>
       <c r="U211" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="212" spans="1:21" x14ac:dyDescent="0.3">
@@ -16706,34 +16664,34 @@
         <v>CT2019_211</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C212" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D212">
         <v>48</v>
       </c>
       <c r="E212" s="3" t="s">
+        <v>777</v>
+      </c>
+      <c r="F212">
+        <v>125</v>
+      </c>
+      <c r="G212" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="H212">
+        <v>48</v>
+      </c>
+      <c r="I212" s="3" t="s">
         <v>778</v>
       </c>
-      <c r="F212">
-        <v>125</v>
-      </c>
-      <c r="G212" s="3" t="s">
+      <c r="J212">
+        <v>125</v>
+      </c>
+      <c r="K212" s="3" t="s">
         <v>795</v>
-      </c>
-      <c r="H212">
-        <v>48</v>
-      </c>
-      <c r="I212" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="J212">
-        <v>125</v>
-      </c>
-      <c r="K212" s="3" t="s">
-        <v>796</v>
       </c>
       <c r="L212" s="3" t="s">
         <v>20</v>
@@ -16763,7 +16721,7 @@
         <v>38</v>
       </c>
       <c r="U212" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="213" spans="1:21" x14ac:dyDescent="0.3">
@@ -16772,34 +16730,34 @@
         <v>CT2019_212</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C213" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D213">
         <v>48</v>
       </c>
       <c r="E213" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="F213">
+        <v>125</v>
+      </c>
+      <c r="G213" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="H213">
+        <v>48</v>
+      </c>
+      <c r="I213" s="3" t="s">
         <v>779</v>
       </c>
-      <c r="F213">
-        <v>125</v>
-      </c>
-      <c r="G213" s="3" t="s">
+      <c r="J213">
+        <v>125</v>
+      </c>
+      <c r="K213" s="3" t="s">
         <v>796</v>
-      </c>
-      <c r="H213">
-        <v>48</v>
-      </c>
-      <c r="I213" s="3" t="s">
-        <v>780</v>
-      </c>
-      <c r="J213">
-        <v>125</v>
-      </c>
-      <c r="K213" s="3" t="s">
-        <v>797</v>
       </c>
       <c r="L213" s="3" t="s">
         <v>240</v>
@@ -16829,7 +16787,7 @@
         <v>40</v>
       </c>
       <c r="U213" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="214" spans="1:21" x14ac:dyDescent="0.3">
@@ -16838,34 +16796,34 @@
         <v>CT2019_213</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C214" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D214">
         <v>48</v>
       </c>
       <c r="E214" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="F214">
+        <v>125</v>
+      </c>
+      <c r="G214" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="H214">
+        <v>48</v>
+      </c>
+      <c r="I214" s="3" t="s">
         <v>780</v>
       </c>
-      <c r="F214">
-        <v>125</v>
-      </c>
-      <c r="G214" s="3" t="s">
+      <c r="J214">
+        <v>125</v>
+      </c>
+      <c r="K214" s="3" t="s">
         <v>797</v>
-      </c>
-      <c r="H214">
-        <v>48</v>
-      </c>
-      <c r="I214" s="3" t="s">
-        <v>781</v>
-      </c>
-      <c r="J214">
-        <v>125</v>
-      </c>
-      <c r="K214" s="3" t="s">
-        <v>798</v>
       </c>
       <c r="L214" s="3" t="s">
         <v>241</v>
@@ -16895,7 +16853,7 @@
         <v>38</v>
       </c>
       <c r="U214" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="215" spans="1:21" x14ac:dyDescent="0.3">
@@ -16904,34 +16862,34 @@
         <v>CT2019_214</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C215" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D215">
         <v>48</v>
       </c>
       <c r="E215" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="F215">
+        <v>125</v>
+      </c>
+      <c r="G215" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="H215">
+        <v>48</v>
+      </c>
+      <c r="I215" s="3" t="s">
         <v>781</v>
       </c>
-      <c r="F215">
-        <v>125</v>
-      </c>
-      <c r="G215" s="3" t="s">
+      <c r="J215">
+        <v>125</v>
+      </c>
+      <c r="K215" s="3" t="s">
         <v>798</v>
-      </c>
-      <c r="H215">
-        <v>48</v>
-      </c>
-      <c r="I215" s="3" t="s">
-        <v>782</v>
-      </c>
-      <c r="J215">
-        <v>125</v>
-      </c>
-      <c r="K215" s="3" t="s">
-        <v>799</v>
       </c>
       <c r="L215" s="3" t="s">
         <v>28</v>
@@ -16961,7 +16919,7 @@
         <v>38</v>
       </c>
       <c r="U215" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="216" spans="1:21" x14ac:dyDescent="0.3">
@@ -16970,34 +16928,34 @@
         <v>CT2019_215</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C216" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D216">
         <v>48</v>
       </c>
       <c r="E216" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="F216">
+        <v>125</v>
+      </c>
+      <c r="G216" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="H216">
+        <v>48</v>
+      </c>
+      <c r="I216" s="3" t="s">
         <v>782</v>
       </c>
-      <c r="F216">
-        <v>125</v>
-      </c>
-      <c r="G216" s="3" t="s">
+      <c r="J216">
+        <v>125</v>
+      </c>
+      <c r="K216" s="3" t="s">
         <v>799</v>
-      </c>
-      <c r="H216">
-        <v>48</v>
-      </c>
-      <c r="I216" s="3" t="s">
-        <v>783</v>
-      </c>
-      <c r="J216">
-        <v>125</v>
-      </c>
-      <c r="K216" s="3" t="s">
-        <v>800</v>
       </c>
       <c r="L216" s="3" t="s">
         <v>182</v>
@@ -17033,34 +16991,34 @@
         <v>CT2019_216</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C217" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D217">
         <v>48</v>
       </c>
       <c r="E217" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="F217">
+        <v>125</v>
+      </c>
+      <c r="G217" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="H217">
+        <v>48</v>
+      </c>
+      <c r="I217" s="3" t="s">
         <v>783</v>
       </c>
-      <c r="F217">
-        <v>125</v>
-      </c>
-      <c r="G217" s="3" t="s">
+      <c r="J217">
+        <v>125</v>
+      </c>
+      <c r="K217" s="3" t="s">
         <v>800</v>
-      </c>
-      <c r="H217">
-        <v>48</v>
-      </c>
-      <c r="I217" s="3" t="s">
-        <v>784</v>
-      </c>
-      <c r="J217">
-        <v>125</v>
-      </c>
-      <c r="K217" s="3" t="s">
-        <v>801</v>
       </c>
       <c r="L217" s="3" t="s">
         <v>101</v>
@@ -17090,7 +17048,7 @@
         <v>74</v>
       </c>
       <c r="U217" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.3">
@@ -17099,34 +17057,34 @@
         <v>CT2019_217</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C218" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D218">
         <v>48</v>
       </c>
       <c r="E218" s="3" t="s">
+        <v>783</v>
+      </c>
+      <c r="F218">
+        <v>125</v>
+      </c>
+      <c r="G218" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="H218">
+        <v>48</v>
+      </c>
+      <c r="I218" s="3" t="s">
         <v>784</v>
       </c>
-      <c r="F218">
-        <v>125</v>
-      </c>
-      <c r="G218" s="3" t="s">
+      <c r="J218">
+        <v>125</v>
+      </c>
+      <c r="K218" s="3" t="s">
         <v>801</v>
-      </c>
-      <c r="H218">
-        <v>48</v>
-      </c>
-      <c r="I218" s="3" t="s">
-        <v>785</v>
-      </c>
-      <c r="J218">
-        <v>125</v>
-      </c>
-      <c r="K218" s="3" t="s">
-        <v>802</v>
       </c>
       <c r="L218" s="3" t="s">
         <v>34</v>
@@ -17156,7 +17114,7 @@
         <v>38</v>
       </c>
       <c r="U218" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.3">
@@ -17165,34 +17123,34 @@
         <v>CT2019_218</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C219" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D219">
         <v>48</v>
       </c>
       <c r="E219" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="F219">
+        <v>125</v>
+      </c>
+      <c r="G219" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="H219">
+        <v>48</v>
+      </c>
+      <c r="I219" s="3" t="s">
         <v>785</v>
       </c>
-      <c r="F219">
-        <v>125</v>
-      </c>
-      <c r="G219" s="3" t="s">
+      <c r="J219">
+        <v>125</v>
+      </c>
+      <c r="K219" s="3" t="s">
         <v>802</v>
-      </c>
-      <c r="H219">
-        <v>48</v>
-      </c>
-      <c r="I219" s="3" t="s">
-        <v>786</v>
-      </c>
-      <c r="J219">
-        <v>125</v>
-      </c>
-      <c r="K219" s="3" t="s">
-        <v>803</v>
       </c>
       <c r="L219" s="3" t="s">
         <v>183</v>
@@ -17222,7 +17180,7 @@
         <v>38</v>
       </c>
       <c r="U219" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="220" spans="1:21" x14ac:dyDescent="0.3">
@@ -17231,34 +17189,34 @@
         <v>CT2019_219</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C220" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D220">
         <v>48</v>
       </c>
       <c r="E220" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="F220">
+        <v>125</v>
+      </c>
+      <c r="G220" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="H220">
+        <v>48</v>
+      </c>
+      <c r="I220" s="3" t="s">
         <v>786</v>
       </c>
-      <c r="F220">
-        <v>125</v>
-      </c>
-      <c r="G220" s="3" t="s">
+      <c r="J220">
+        <v>125</v>
+      </c>
+      <c r="K220" s="3" t="s">
         <v>803</v>
-      </c>
-      <c r="H220">
-        <v>48</v>
-      </c>
-      <c r="I220" s="3" t="s">
-        <v>787</v>
-      </c>
-      <c r="J220">
-        <v>125</v>
-      </c>
-      <c r="K220" s="3" t="s">
-        <v>804</v>
       </c>
       <c r="L220" s="3" t="s">
         <v>184</v>
@@ -17288,7 +17246,7 @@
         <v>38</v>
       </c>
       <c r="U220" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="221" spans="1:21" x14ac:dyDescent="0.3">
@@ -17297,34 +17255,34 @@
         <v>CT2019_220</v>
       </c>
       <c r="B221" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="C221" t="s">
         <v>770</v>
       </c>
-      <c r="C221" t="s">
-        <v>771</v>
-      </c>
       <c r="D221">
         <v>48</v>
       </c>
       <c r="E221" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="F221">
+        <v>125</v>
+      </c>
+      <c r="G221" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="H221">
+        <v>48</v>
+      </c>
+      <c r="I221" s="3" t="s">
         <v>787</v>
       </c>
-      <c r="F221">
-        <v>125</v>
-      </c>
-      <c r="G221" s="3" t="s">
+      <c r="J221">
+        <v>125</v>
+      </c>
+      <c r="K221" s="3" t="s">
         <v>804</v>
-      </c>
-      <c r="H221">
-        <v>48</v>
-      </c>
-      <c r="I221" s="3" t="s">
-        <v>788</v>
-      </c>
-      <c r="J221">
-        <v>125</v>
-      </c>
-      <c r="K221" s="3" t="s">
-        <v>805</v>
       </c>
       <c r="L221" s="3" t="s">
         <v>44</v>
@@ -17354,7 +17312,7 @@
         <v>38</v>
       </c>
       <c r="U221" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>